<commit_message>
Added MyConstructor for changing typical parameters
</commit_message>
<xml_diff>
--- a/MacV1Buildup/tables/PC_apical_dendrites.xlsx
+++ b/MacV1Buildup/tables/PC_apical_dendrites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simo\Laskenta\Git_Repos\CxConstructor\MacV1Buildup\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A2D0BA-EBC0-44ED-AB9E-D4444B7F35E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724A750-F6F8-49B8-B0AF-0E7198DB6C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D7AC558D-2DAE-4BAC-9877-0C40EC01BC08}"/>
+    <workbookView xWindow="30630" yWindow="1830" windowWidth="12150" windowHeight="20775" xr2:uid="{D7AC558D-2DAE-4BAC-9877-0C40EC01BC08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>layer</t>
   </si>
@@ -117,6 +117,30 @@
   </si>
   <si>
     <t>L4CB</t>
+  </si>
+  <si>
+    <t>No pyramidal cells in monkeys, but here for technical reasons/other species</t>
+  </si>
+  <si>
+    <t>[L4CA-&gt;L1]</t>
+  </si>
+  <si>
+    <t>[L4CA-&gt;L23]</t>
+  </si>
+  <si>
+    <t>[L4CB-&gt;L1]</t>
+  </si>
+  <si>
+    <t>[L4CB-&gt;L23]</t>
+  </si>
+  <si>
+    <t>L4C</t>
+  </si>
+  <si>
+    <t>[L4C-&gt;L1]</t>
+  </si>
+  <si>
+    <t>[L4C-&gt;L23]</t>
   </si>
 </sst>
 </file>
@@ -469,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E048E46-E608-477C-9EFA-1AD3E55155F3}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,13 +570,13 @@
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -560,10 +584,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -571,29 +595,43 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>